<commit_message>
config, static, bug: 'bat in windows' statement added to readme, date column corrected in program xlsx, initial lang session state variable creation added to every page
</commit_message>
<xml_diff>
--- a/static/xlsx/Program.xlsx
+++ b/static/xlsx/Program.xlsx
@@ -25,58 +25,64 @@
     <t>Link</t>
   </si>
   <si>
+    <t>Microsoft Imagine</t>
+  </si>
+  <si>
+    <t>https://bidb.iyte.edu.tr/microsoft-imagine-academy/</t>
+  </si>
+  <si>
+    <t>Aspire Leaders</t>
+  </si>
+  <si>
+    <t>https://apply.aspireleaders.org/f/64413a183b5d0038f900087e</t>
+  </si>
+  <si>
+    <t>Başlangıç Noktası Akademi</t>
+  </si>
+  <si>
+    <t>https://akademi.baslangicnoktasi.org/</t>
+  </si>
+  <si>
+    <t>LEAD21 Fellowship</t>
+  </si>
+  <si>
+    <t>https://www.youthall.com/tr/yenibirlider/lead21-fellowship-programi_7/</t>
+  </si>
+  <si>
+    <t>McKinsey Forward</t>
+  </si>
+  <si>
+    <t>https://www.mckinsey.com/forward/regions/turkey-and-azerbaijan</t>
+  </si>
+  <si>
+    <t>Koç Ctrl+ Future</t>
+  </si>
+  <si>
+    <t>https://www.kockariyerim.com/jobAds/koc-toplulugu-sirketleri-ctrl-future-programi/0d41fa03-0bc5-4ba3-b272-8f161a71b238</t>
+  </si>
+  <si>
+    <t>Akbank Fellowship</t>
+  </si>
+  <si>
+    <t>https://form.jotform.com/231551887039968</t>
+  </si>
+  <si>
     <t>Girvak Fellow</t>
   </si>
   <si>
     <t>https://girvak.bonapply.com/</t>
   </si>
   <si>
-    <t>McKinsey Forward</t>
-  </si>
-  <si>
-    <t>https://www.mckinsey.com/forward/regions/turkey-and-azerbaijan</t>
-  </si>
-  <si>
-    <t>LEAD21 Fellowship</t>
-  </si>
-  <si>
-    <t>https://www.youthall.com/tr/yenibirlider/lead21-fellowship-programi_7/</t>
-  </si>
-  <si>
-    <t>Koç Ctrl+ Future</t>
-  </si>
-  <si>
-    <t>https://www.kockariyerim.com/jobAds/koc-toplulugu-sirketleri-ctrl-future-programi/0d41fa03-0bc5-4ba3-b272-8f161a71b238</t>
-  </si>
-  <si>
-    <t>Akbank Fellowship</t>
-  </si>
-  <si>
-    <t>https://form.jotform.com/231551887039968</t>
-  </si>
-  <si>
-    <t>Aspire Leaders</t>
-  </si>
-  <si>
-    <t>https://apply.aspireleaders.org/f/64413a183b5d0038f900087e</t>
-  </si>
-  <si>
     <t>GDSC Leads</t>
   </si>
   <si>
     <t>https://developers.google.com/community/gdsc/leads</t>
   </si>
   <si>
-    <t>Microsoft Imagine</t>
-  </si>
-  <si>
-    <t>https://bidb.iyte.edu.tr/microsoft-imagine-academy/</t>
-  </si>
-  <si>
-    <t>Başlangıç Noktası Akademi</t>
-  </si>
-  <si>
-    <t>https://akademi.baslangicnoktasi.org/</t>
+    <t>DevPaths</t>
+  </si>
+  <si>
+    <t>https://kesisenyollar.org/devpaths/</t>
   </si>
   <si>
     <t>Yetkin Gençler</t>
@@ -85,10 +91,16 @@
     <t>https://airtable.com/shrjRQI3DjWuGQuyO</t>
   </si>
   <si>
-    <t>DevPaths</t>
-  </si>
-  <si>
-    <t>https://kesisenyollar.org/devpaths/</t>
+    <t>Fintek Çırağı Programı</t>
+  </si>
+  <si>
+    <t>https://www.todeb.org.tr/detay/fintek-ciragi-programi-icerik/459/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gelecek Vadeden Girişimler </t>
+  </si>
+  <si>
+    <t>https://gelecekvadedenler.com/</t>
   </si>
   <si>
     <t>Google Oyun Akademisi</t>
@@ -101,18 +113,6 @@
   </si>
   <si>
     <t>https://techxtile.net/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gelecek Vadeden Girişimler </t>
-  </si>
-  <si>
-    <t>https://gelecekvadedenler.com/</t>
-  </si>
-  <si>
-    <t>Fintek Çırağı Programı</t>
-  </si>
-  <si>
-    <t>https://www.todeb.org.tr/detay/fintek-ciragi-programi-icerik/459/</t>
   </si>
 </sst>
 </file>
@@ -126,7 +126,7 @@
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="m/d/yyyy;@"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,13 +153,6 @@
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -609,152 +602,152 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -763,7 +756,10 @@
     <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="58" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1084,17 +1080,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B$1:B$1048576"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="28.7777777777778" customWidth="1"/>
     <col min="2" max="2" width="19.2222222222222" style="1" customWidth="1"/>
-    <col min="3" max="3" width="104.555555555556" customWidth="1"/>
+    <col min="3" max="3" width="15.7777777777778" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1126,7 +1122,7 @@
       <c r="B3" s="5">
         <v>44937</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1137,7 +1133,7 @@
       <c r="B4" s="5">
         <v>45016</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1148,7 +1144,7 @@
       <c r="B5" s="5">
         <v>45096</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1159,7 +1155,7 @@
       <c r="B6" s="5">
         <v>45097</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1170,7 +1166,7 @@
       <c r="B7" s="5">
         <v>45109</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1181,7 +1177,7 @@
       <c r="B8" s="5">
         <v>45109</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1203,7 +1199,7 @@
       <c r="B10" s="5">
         <v>45121</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1214,7 +1210,7 @@
       <c r="B11" s="5">
         <v>45121</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1225,7 +1221,7 @@
       <c r="B12" s="5">
         <v>45125</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="6" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1236,7 +1232,7 @@
       <c r="B13" s="5">
         <v>45190</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1247,7 +1243,7 @@
       <c r="B14" s="5">
         <v>45199</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="4" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1258,7 +1254,7 @@
       <c r="B15" s="5">
         <v>45214</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="6" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1269,13 +1265,76 @@
       <c r="B16" s="5">
         <v>45214</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="6" t="s">
         <v>32</v>
       </c>
     </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="8"/>
+      <c r="B19" s="9"/>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="8"/>
+      <c r="B20" s="10"/>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="8"/>
+      <c r="B21" s="10"/>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="8"/>
+      <c r="B22" s="10"/>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="8"/>
+      <c r="B23" s="10"/>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="8"/>
+      <c r="B24" s="10"/>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="8"/>
+      <c r="B25" s="10"/>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="8"/>
+      <c r="B26" s="10"/>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="8"/>
+      <c r="B27" s="10"/>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="8"/>
+      <c r="B28" s="10"/>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="8"/>
+      <c r="B29" s="10"/>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="8"/>
+      <c r="B30" s="10"/>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="8"/>
+      <c r="B31" s="10"/>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="8"/>
+      <c r="B32" s="8"/>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="8"/>
+      <c r="B33" s="10"/>
+    </row>
   </sheetData>
+  <sortState ref="A2:C16">
+    <sortCondition ref="B2:B16"/>
+  </sortState>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="https://girvak.bonapply.com/"/>
+    <hyperlink ref="C9" r:id="rId1" display="https://girvak.bonapply.com/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>